<commit_message>
Adding Tom to excel
</commit_message>
<xml_diff>
--- a/userCfg.xlsx
+++ b/userCfg.xlsx
@@ -2,19 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="10560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Emre" sheetId="1" r:id="rId1"/>
     <sheet name="Jan" sheetId="2" r:id="rId2"/>
-    <sheet name="Em" r:id="rId6" sheetId="3"/>
+    <sheet name="Em" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -66,8 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,7 +106,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -394,8 +392,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,8 +443,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -495,13 +493,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
*fixing the pc config of people (excel)
TO DO:
-New user make verification: yes/no
-greyout everything except login when user isn't logged in yet
</commit_message>
<xml_diff>
--- a/userCfg.xlsx
+++ b/userCfg.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="10560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="10560" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Emre" sheetId="1" r:id="rId1"/>
-    <sheet name="Jan" sheetId="2" r:id="rId2"/>
-    <sheet name="Em" sheetId="3" r:id="rId3"/>
+    <sheet name="emre" sheetId="1" r:id="rId1"/>
+    <sheet name="jan" sheetId="2" r:id="rId2"/>
+    <sheet name="tom" sheetId="3" r:id="rId3"/>
+    <sheet name="fvjhtjhtjht" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>nameComponent</t>
   </si>
@@ -61,11 +62,15 @@
   <si>
     <t>groupComponent</t>
   </si>
+  <si>
+    <t>GEL316GB1600C9DC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,7 +111,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,8 +397,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -437,14 +442,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -494,12 +499,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Before calculate watt usage fix
</commit_message>
<xml_diff>
--- a/userCfg.xlsx
+++ b/userCfg.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="10560" activeTab="2"/>
   </bookViews>
@@ -10,7 +10,6 @@
     <sheet name="emre" sheetId="1" r:id="rId1"/>
     <sheet name="jan" sheetId="2" r:id="rId2"/>
     <sheet name="tom" sheetId="3" r:id="rId3"/>
-    <sheet name="fvjhtjhtjht" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>nameComponent</t>
   </si>
@@ -64,12 +63,27 @@
   </si>
   <si>
     <t>GEL316GB1600C9DC</t>
+  </si>
+  <si>
+    <t>GTX Titan X</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">950 EVO </t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>G550M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -111,7 +125,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,7 +466,7 @@
     <col min="2" max="2" customWidth="true" width="23.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -460,7 +474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -468,7 +482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -476,20 +490,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -499,7 +529,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -529,28 +559,15 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
1. autosave user cfg when exiting application 2. verification text boxes replaced by only 1 (String input like error box) 3. adding clear button to compare tab 4. cleaning A LOT OF CODE including warnings. 5. Fix search
</commit_message>
<xml_diff>
--- a/userCfg.xlsx
+++ b/userCfg.xlsx
@@ -11,6 +11,7 @@
     <sheet name="tom" sheetId="3" r:id="rId3"/>
     <sheet name="notworking" sheetId="4" r:id="rId4"/>
     <sheet name="jan" r:id="rId8" sheetId="5"/>
+    <sheet name="thomas" r:id="rId9" sheetId="6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="27">
   <si>
     <t>nameComponent</t>
   </si>
@@ -91,6 +92,18 @@
   </si>
   <si>
     <t>950 EVO</t>
+  </si>
+  <si>
+    <t>i7 5960X</t>
+  </si>
+  <si>
+    <t>970 Gaming</t>
+  </si>
+  <si>
+    <t>Dark Power Pro 11</t>
+  </si>
+  <si>
+    <t>MAXIMUS VII RANGER</t>
   </si>
 </sst>
 </file>
@@ -639,4 +652,73 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>